<commit_message>
Fixed readme and sample code
</commit_message>
<xml_diff>
--- a/samples/people.xlsx
+++ b/samples/people.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{045375D8-B3EF-E644-B165-C1B0EDEA7E7E}"/>
+    <workbookView xWindow="9660" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{045375D8-B3EF-E644-B165-C1B0EDEA7E7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>Full Name</t>
   </si>
@@ -141,6 +141,36 @@
   </si>
   <si>
     <t>65 inches</t>
+  </si>
+  <si>
+    <t>Federico Carusso</t>
+  </si>
+  <si>
+    <t>carusso@test.test</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>1966.09.15</t>
+  </si>
+  <si>
+    <t>Italia</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Sicilia</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Pasta 8888</t>
+  </si>
+  <si>
+    <t>75 inches</t>
   </si>
 </sst>
 </file>
@@ -503,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08922F5D-3916-CB49-9EFB-5D7F8FDCA0BF}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,11 +713,53 @@
         <v>38</v>
       </c>
     </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5">
+        <v>5555555</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="K5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5">
+        <v>22222</v>
+      </c>
+      <c r="M5" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{C34477E7-F237-044C-A120-5F8F4641386D}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{3B563163-AAF4-3249-BBD8-183DA4048E34}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{A6DA13A4-D388-EC44-8D8E-A725DB2F697F}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{3A6B4DF9-A210-2248-8BE2-60B4AC1341BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>